<commit_message>
Complete RHI plot for Exp 2
</commit_message>
<xml_diff>
--- a/Processing/Exp2_delay.xlsx
+++ b/Processing/Exp2_delay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIBS\Documents\Documents\SOPHy_Calibration\Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976DEC2D-0632-4BB0-A58D-43EBEF1A0669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A54B87-E292-4208-A6D4-B4055080D028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -816,14 +816,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="40.6328125" customWidth="1"/>
-    <col min="3" max="3" width="46.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
     <col min="4" max="5" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>